<commit_message>
add comments to participant order sheet
</commit_message>
<xml_diff>
--- a/res/participant_order.xlsx
+++ b/res/participant_order.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annebelle/Documents/GitHub/MAIR-group12/res/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20D9D7F-D81B-0140-AEDD-E0C1175100B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet 1 - Participant order of "/>
+    <sheet name="Sheet 1 - Participant order of " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="23">
   <si>
     <t>Participant number</t>
   </si>
@@ -50,13 +56,45 @@
   </si>
   <si>
     <t>Informal</t>
+  </si>
+  <si>
+    <t>done by</t>
+  </si>
+  <si>
+    <t>annebelle</t>
+  </si>
+  <si>
+    <t>robin</t>
+  </si>
+  <si>
+    <t>ellora</t>
+  </si>
+  <si>
+    <t>tomas</t>
+  </si>
+  <si>
+    <t>ellora?</t>
+  </si>
+  <si>
+    <t>json?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>drop older version of 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,12 +125,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000ff"/>
+        <fgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -106,106 +144,106 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </right>
       <top style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </left>
       <right style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </right>
       <top style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF00ff00"/>
+        <color rgb="FF00FF00"/>
       </left>
       <right style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </right>
       <top style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -213,50 +251,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -267,10 +305,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="5E5E5E"/>
@@ -308,71 +346,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,7 +438,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -423,11 +461,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -436,13 +474,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -452,7 +490,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -461,7 +499,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -470,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -478,10 +516,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -546,29 +584,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="16.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -593,8 +628,17 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -619,8 +663,14 @@
       <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -645,8 +695,14 @@
       <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -671,8 +727,14 @@
       <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -697,8 +759,17 @@
       <c r="H5" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -723,8 +794,14 @@
       <c r="H6" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -749,8 +826,14 @@
       <c r="H7" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -775,8 +858,14 @@
       <c r="H8" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -801,8 +890,14 @@
       <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -827,8 +922,14 @@
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -853,8 +954,14 @@
       <c r="H11" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -879,8 +986,14 @@
       <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -905,8 +1018,14 @@
       <c r="H13" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -931,8 +1050,14 @@
       <c r="H14" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="I14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -957,8 +1082,14 @@
       <c r="H15" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -984,7 +1115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1010,7 +1141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1036,7 +1167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1062,7 +1193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1087,8 +1218,14 @@
       <c r="H20" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1113,8 +1250,14 @@
       <c r="H21" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1139,8 +1282,14 @@
       <c r="H22" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1166,7 +1315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1191,8 +1340,14 @@
       <c r="H24" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1217,8 +1372,14 @@
       <c r="H25" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -1243,8 +1404,14 @@
       <c r="H26" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1269,8 +1436,14 @@
       <c r="H27" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -1295,8 +1468,14 @@
       <c r="H28" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.05" customFormat="1" s="1">
+      <c r="I28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1322,7 +1501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1348,7 +1527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -1374,7 +1553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -1400,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.05" customFormat="1" s="1">
+    <row r="33" spans="1:8" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>

</xml_diff>